<commit_message>
International imports redone using a commodity merchandise database. Still need validation by comparing to Exiobase emissions level. Also, the import merchandise file is too big for Github, need to think of something.
</commit_message>
<xml_diff>
--- a/Data/IOIC_EXIOBASE.xlsx
+++ b/Data/IOIC_EXIOBASE.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25427"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25601"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\11max\PycharmProjects\OpenIOCanada\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFEDAAAE-30A6-4C98-92F7-38735BB3783A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7463EEC-B317-4EE0-8D5B-B6083C2ED4A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -12441,10 +12441,10 @@
   <dimension ref="A1:GT495"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="DN298" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C197" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="DY315" sqref="DY315"/>
+      <selection pane="bottomRight" activeCell="A207" sqref="A207"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -15913,7 +15913,7 @@
       <c r="B135" s="4" t="s">
         <v>1764</v>
       </c>
-      <c r="BI135">
+      <c r="BH135">
         <v>1</v>
       </c>
     </row>
@@ -16023,7 +16023,7 @@
       <c r="B145" s="4" t="s">
         <v>1784</v>
       </c>
-      <c r="BK145">
+      <c r="BL145">
         <v>1</v>
       </c>
     </row>
@@ -16491,7 +16491,7 @@
       <c r="B184" s="4" t="s">
         <v>1862</v>
       </c>
-      <c r="CK184">
+      <c r="CJ184">
         <v>1</v>
       </c>
     </row>
@@ -16560,7 +16560,7 @@
       <c r="B190" s="4" t="s">
         <v>1874</v>
       </c>
-      <c r="CV190">
+      <c r="CU190">
         <v>1</v>
       </c>
     </row>
@@ -16586,7 +16586,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="193" spans="1:118" x14ac:dyDescent="0.3">
+    <row r="193" spans="1:119" x14ac:dyDescent="0.3">
       <c r="A193" s="4" t="s">
         <v>1879</v>
       </c>
@@ -16597,7 +16597,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="194" spans="1:118" x14ac:dyDescent="0.3">
+    <row r="194" spans="1:119" x14ac:dyDescent="0.3">
       <c r="A194" s="4" t="s">
         <v>1881</v>
       </c>
@@ -16608,7 +16608,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="195" spans="1:118" x14ac:dyDescent="0.3">
+    <row r="195" spans="1:119" x14ac:dyDescent="0.3">
       <c r="A195" s="4" t="s">
         <v>1883</v>
       </c>
@@ -16619,7 +16619,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="196" spans="1:118" x14ac:dyDescent="0.3">
+    <row r="196" spans="1:119" x14ac:dyDescent="0.3">
       <c r="A196" s="4" t="s">
         <v>1885</v>
       </c>
@@ -16630,7 +16630,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="197" spans="1:118" x14ac:dyDescent="0.3">
+    <row r="197" spans="1:119" x14ac:dyDescent="0.3">
       <c r="A197" s="4" t="s">
         <v>1887</v>
       </c>
@@ -16641,7 +16641,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="198" spans="1:118" x14ac:dyDescent="0.3">
+    <row r="198" spans="1:119" x14ac:dyDescent="0.3">
       <c r="A198" s="4" t="s">
         <v>1889</v>
       </c>
@@ -16652,7 +16652,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="199" spans="1:118" x14ac:dyDescent="0.3">
+    <row r="199" spans="1:119" x14ac:dyDescent="0.3">
       <c r="A199" s="4" t="s">
         <v>1891</v>
       </c>
@@ -16663,7 +16663,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="200" spans="1:118" x14ac:dyDescent="0.3">
+    <row r="200" spans="1:119" x14ac:dyDescent="0.3">
       <c r="A200" s="4" t="s">
         <v>1893</v>
       </c>
@@ -16674,7 +16674,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="201" spans="1:118" x14ac:dyDescent="0.3">
+    <row r="201" spans="1:119" x14ac:dyDescent="0.3">
       <c r="A201" s="4" t="s">
         <v>1895</v>
       </c>
@@ -16685,7 +16685,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="202" spans="1:118" x14ac:dyDescent="0.3">
+    <row r="202" spans="1:119" x14ac:dyDescent="0.3">
       <c r="A202" s="4" t="s">
         <v>1897</v>
       </c>
@@ -16696,7 +16696,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="203" spans="1:118" x14ac:dyDescent="0.3">
+    <row r="203" spans="1:119" x14ac:dyDescent="0.3">
       <c r="A203" s="4" t="s">
         <v>1899</v>
       </c>
@@ -16707,7 +16707,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="204" spans="1:118" x14ac:dyDescent="0.3">
+    <row r="204" spans="1:119" x14ac:dyDescent="0.3">
       <c r="A204" s="4" t="s">
         <v>1901</v>
       </c>
@@ -16718,47 +16718,47 @@
         <v>1</v>
       </c>
     </row>
-    <row r="205" spans="1:118" x14ac:dyDescent="0.3">
+    <row r="205" spans="1:119" x14ac:dyDescent="0.3">
       <c r="A205" s="4" t="s">
         <v>1903</v>
       </c>
       <c r="B205" s="4" t="s">
         <v>1904</v>
       </c>
-      <c r="DN205">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="206" spans="1:118" x14ac:dyDescent="0.3">
+      <c r="DO205">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="206" spans="1:119" x14ac:dyDescent="0.3">
       <c r="A206" s="4" t="s">
         <v>1905</v>
       </c>
       <c r="B206" s="4" t="s">
         <v>1906</v>
       </c>
-      <c r="DN206">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="207" spans="1:118" x14ac:dyDescent="0.3">
+      <c r="DO206">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="207" spans="1:119" x14ac:dyDescent="0.3">
       <c r="A207" s="4" t="s">
         <v>1907</v>
       </c>
       <c r="B207" s="4" t="s">
         <v>1908</v>
       </c>
-      <c r="DC207">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="208" spans="1:118" x14ac:dyDescent="0.3">
+      <c r="DB207">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="208" spans="1:119" x14ac:dyDescent="0.3">
       <c r="A208" s="4" t="s">
         <v>1909</v>
       </c>
       <c r="B208" s="4" t="s">
         <v>1910</v>
       </c>
-      <c r="DM208">
+      <c r="DL208">
         <v>1</v>
       </c>
     </row>
@@ -17703,6 +17703,9 @@
       </c>
       <c r="B294" s="4" t="s">
         <v>2081</v>
+      </c>
+      <c r="DN294">
+        <v>1</v>
       </c>
       <c r="DW294">
         <v>1</v>

</xml_diff>

<commit_message>
Correction for Latvia Patent fuel import by Nova Scotia going crazy because of Exiobase emission factor.
</commit_message>
<xml_diff>
--- a/Data/IOIC_EXIOBASE.xlsx
+++ b/Data/IOIC_EXIOBASE.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25629"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\11max\PycharmProjects\OpenIOCanada\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7463EEC-B317-4EE0-8D5B-B6083C2ED4A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D3DF86C-5F3B-4F17-AF22-DC44C2B0C7B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -12441,10 +12441,10 @@
   <dimension ref="A1:GT495"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C197" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="R19" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="A207" sqref="A207"/>
+      <selection pane="bottomRight" activeCell="Y25" sqref="Y25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -14710,9 +14710,6 @@
       <c r="Y37">
         <v>1</v>
       </c>
-      <c r="Z37">
-        <v>1</v>
-      </c>
       <c r="AA37">
         <v>1</v>
       </c>
@@ -14893,9 +14890,6 @@
         <v>1</v>
       </c>
       <c r="Y51">
-        <v>1</v>
-      </c>
-      <c r="Z51">
         <v>1</v>
       </c>
       <c r="AA51">

</xml_diff>